<commit_message>
inhancement in the code.
</commit_message>
<xml_diff>
--- a/KEM_Tool/testdata/Users.xlsx
+++ b/KEM_Tool/testdata/Users.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kaiser Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akshay.Bokan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>kaiser.sme@gmail.com</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>kaiser.requestor@gmail.com</t>
+  </si>
+  <si>
+    <t>aba123@gmail.com</t>
+  </si>
+  <si>
+    <t>322aas</t>
   </si>
 </sst>
 </file>
@@ -401,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +467,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -469,8 +483,9 @@
     <hyperlink ref="A4" r:id="rId4"/>
     <hyperlink ref="A5" r:id="rId5"/>
     <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A7" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>